<commit_message>
PMO-2298: fixed aad/aal and special cases of loss carried forward situations
</commit_message>
<xml_diff>
--- a/test/data/spreadsheets/PMO-2198_a___SSC_usual_3.xlsx
+++ b/test/data/spreadsheets/PMO-2198_a___SSC_usual_3.xlsx
@@ -993,7 +993,7 @@
     <numFmt numFmtId="168" formatCode="#,##0;\-#,##0;"/>
     <numFmt numFmtId="169" formatCode="#,##0;\-#,##0;0"/>
     <numFmt numFmtId="170" formatCode="#,##0.0000;\-#,##0.0000;0.0000"/>
-    <numFmt numFmtId="176" formatCode="#,##0.0000000;\-#,##0.0000000;0.0000000"/>
+    <numFmt numFmtId="171" formatCode="#,##0.0000000;\-#,##0.0000000;0.0000000"/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -1780,7 +1780,7 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="170" fontId="14" fillId="10" borderId="6" xfId="3" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="14" fillId="10" borderId="6" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="14" fillId="10" borderId="6" xfId="3" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -2450,25 +2450,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="117293824"/>
-        <c:axId val="117391360"/>
+        <c:axId val="113966080"/>
+        <c:axId val="114033408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="117293824"/>
+        <c:axId val="113966080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117391360"/>
+        <c:crossAx val="114033408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="117391360"/>
+        <c:axId val="114033408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2476,7 +2476,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117293824"/>
+        <c:crossAx val="113966080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2488,7 +2488,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2770,11 +2770,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="59737984"/>
-        <c:axId val="117393664"/>
+        <c:axId val="114128768"/>
+        <c:axId val="114130944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="59737984"/>
+        <c:axId val="114128768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2795,16 +2795,17 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117393664"/>
+        <c:crossAx val="114130944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="117393664"/>
+        <c:axId val="114130944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2826,10 +2827,11 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59737984"/>
+        <c:crossAx val="114128768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5450,7 +5452,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AY287"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A163" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C209" sqref="C209"/>
     </sheetView>
   </sheetViews>
@@ -6524,7 +6526,7 @@
         <v>8.699999999999998E-2</v>
       </c>
       <c r="C63" s="192">
-        <f t="dataTable" ref="C63:F63" dt2D="0" dtr="1" r1="D57"/>
+        <f t="dataTable" ref="C63:F63" dt2D="0" dtr="1" r1="D57" ca="1"/>
         <v>4.349999999999999E-2</v>
       </c>
       <c r="D63" s="192">
@@ -6570,7 +6572,7 @@
         <v>8.699999999999998E-2</v>
       </c>
       <c r="C65" s="126">
-        <f t="dataTable" ref="C65:F65" dt2D="0" dtr="1" r1="D57" ca="1"/>
+        <f t="dataTable" ref="C65:F65" dt2D="0" dtr="1" r1="D57"/>
         <v>0</v>
       </c>
       <c r="D65" s="192">
@@ -7337,7 +7339,7 @@
         <v>0.17999999999999994</v>
       </c>
       <c r="J102" s="126">
-        <f t="dataTable" ref="J102:AY102" dt2D="0" dtr="1" r1="D105"/>
+        <f t="dataTable" ref="J102:AY102" dt2D="0" dtr="1" r1="D105" ca="1"/>
         <v>0.9</v>
       </c>
       <c r="K102" s="126">
@@ -7737,7 +7739,7 @@
         <v>0.17999999999999994</v>
       </c>
       <c r="C118" s="192">
-        <f t="dataTable" ref="C118:F118" dt2D="0" dtr="1" r1="D105" ca="1"/>
+        <f t="dataTable" ref="C118:F118" dt2D="0" dtr="1" r1="D105"/>
         <v>0.45284999999999997</v>
       </c>
       <c r="D118" s="192">

</xml_diff>